<commit_message>
update BOM for Expansion Board
</commit_message>
<xml_diff>
--- a/hw/EXP1802 BOM.xlsx
+++ b/hw/EXP1802 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fours\Documents\SBC1802\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwasson/Development/awasson/SBC1802/hw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0486C885-84CB-4867-A778-8A53008C37D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9232A4FA-A18F-794B-89BA-706878BC5DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="270" windowWidth="17930" windowHeight="10530" xr2:uid="{E6317DB6-1395-40AB-B574-B66DE8210E28}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="29960" windowHeight="25460" xr2:uid="{E6317DB6-1395-40AB-B574-B66DE8210E28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="181">
   <si>
     <t>Qty</t>
   </si>
@@ -139,9 +139,6 @@
     <t>MAX232N</t>
   </si>
   <si>
-    <t>U16</t>
-  </si>
-  <si>
     <t>74HC245</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>10k Ohms</t>
   </si>
   <si>
-    <t>1uF</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -376,21 +370,6 @@
     <t>2x5,10 Pin, Male,Shrouded Header</t>
   </si>
   <si>
-    <t>U1,U9</t>
-  </si>
-  <si>
-    <t>CDP1855</t>
-  </si>
-  <si>
-    <t>CDP1855CE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8-Bit Prog Multiply/Divide</t>
-  </si>
-  <si>
-    <t>U3,U4</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
@@ -418,9 +397,6 @@
     <t>Dual Counter Timer</t>
   </si>
   <si>
-    <t>U10,U13,U17</t>
-  </si>
-  <si>
     <t>CDP1851</t>
   </si>
   <si>
@@ -436,12 +412,6 @@
     <t>74HC125</t>
   </si>
   <si>
-    <t>U14,U15</t>
-  </si>
-  <si>
-    <t>U11,U12</t>
-  </si>
-  <si>
     <t>AY-3-8912</t>
   </si>
   <si>
@@ -463,15 +433,9 @@
     <t>AY-3-8912A</t>
   </si>
   <si>
-    <t>R1,R2,R4,R5,R10</t>
-  </si>
-  <si>
     <t>1k Ohms</t>
   </si>
   <si>
-    <t>R6,R9,R11</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -481,9 +445,6 @@
     <t>CF18JT1K00</t>
   </si>
   <si>
-    <t>R7,R8</t>
-  </si>
-  <si>
     <t>CF18JT2K20CT-ND</t>
   </si>
   <si>
@@ -493,24 +454,9 @@
     <t>CF18JT2K20</t>
   </si>
   <si>
-    <t>RP1,RP2</t>
-  </si>
-  <si>
-    <t>C1,C2,C3,C4</t>
-  </si>
-  <si>
-    <t>C10-C25</t>
-  </si>
-  <si>
     <t>C5</t>
   </si>
   <si>
-    <t>100uF</t>
-  </si>
-  <si>
-    <t>C6,C7</t>
-  </si>
-  <si>
     <t>TAP107K020CCS</t>
   </si>
   <si>
@@ -520,15 +466,6 @@
     <t>LED1</t>
   </si>
   <si>
-    <t>U10,U11,U12,U13,U17</t>
-  </si>
-  <si>
-    <t>U2,U5,U6</t>
-  </si>
-  <si>
-    <t>U3,U4,U8,U16</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -581,6 +518,66 @@
   </si>
   <si>
     <t>Audio Jack Stereo (TRS), 3.5mm,R/A</t>
+  </si>
+  <si>
+    <t>U16, U18</t>
+  </si>
+  <si>
+    <t>U10, U17</t>
+  </si>
+  <si>
+    <t>U11, U12</t>
+  </si>
+  <si>
+    <t>U14, U15</t>
+  </si>
+  <si>
+    <t>R1, R2, R4, R5, R12, R13, R14, R15</t>
+  </si>
+  <si>
+    <t>R6, R9, R10, R11</t>
+  </si>
+  <si>
+    <t>RP1, RP2,  RP3</t>
+  </si>
+  <si>
+    <t>R7, R8</t>
+  </si>
+  <si>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t>4.7nf</t>
+  </si>
+  <si>
+    <t>Capacitor, Ceramic Mono, 4.7nF"</t>
+  </si>
+  <si>
+    <t>C8, C9</t>
+  </si>
+  <si>
+    <t>C6, C7</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4</t>
+  </si>
+  <si>
+    <t>U10, U11, U12, U17</t>
+  </si>
+  <si>
+    <t>U2, U5, U6</t>
+  </si>
+  <si>
+    <t>U1, U9</t>
+  </si>
+  <si>
+    <t>U8, U16, 18</t>
+  </si>
+  <si>
+    <t>C10 - C23</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -642,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -675,6 +672,9 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,28 +1000,28 @@
   <dimension ref="A2:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
-    <col min="3" max="3" width="34.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="34.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1047,11 +1047,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1073,11 +1073,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1100,18 +1100,18 @@
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>116</v>
+        <v>1</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -1120,108 +1120,108 @@
         <v>115</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>120</v>
+      <c r="B7" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>119</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>122</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>22</v>
+      <c r="B8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>23</v>
+      <c r="B9" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>118</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
-        <v>124</v>
+      <c r="B10" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -1230,445 +1230,436 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>128</v>
+        <v>2</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>131</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="F12" t="s">
-        <v>41</v>
+      <c r="F12" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
-        <v>132</v>
+      <c r="B13" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>140</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>137</v>
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
-        <v>35</v>
+      <c r="B14" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>37</v>
+        <v>129</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" t="s">
+        <v>131</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
         <v>133</v>
       </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>168</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="B24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
         <v>139</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>173</v>
+      </c>
+      <c r="E25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="G15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" t="s">
-        <v>142</v>
-      </c>
-      <c r="E19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" t="s">
-        <v>145</v>
-      </c>
-      <c r="E20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>143</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" t="s">
-        <v>144</v>
-      </c>
-      <c r="E21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>146</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" t="s">
-        <v>148</v>
-      </c>
-      <c r="E22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" t="s">
-        <v>151</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" t="s">
-        <v>152</v>
-      </c>
-      <c r="E23" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>4</v>
-      </c>
-      <c r="B24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" t="s">
-        <v>153</v>
-      </c>
-      <c r="E24" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" t="s">
-        <v>155</v>
-      </c>
-      <c r="E25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
-      <c r="B26" t="s">
-        <v>156</v>
+      <c r="B26" s="12" t="s">
+        <v>170</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>66</v>
+        <v>171</v>
       </c>
       <c r="D26" t="s">
-        <v>157</v>
-      </c>
-      <c r="E26" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>16</v>
-      </c>
-      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="D27" t="s">
+        <v>179</v>
+      </c>
+      <c r="E27" t="s">
         <v>62</v>
       </c>
-      <c r="D27" t="s">
-        <v>154</v>
-      </c>
-      <c r="E27" t="s">
-        <v>64</v>
-      </c>
       <c r="F27" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
-      <c r="B28" t="s">
-        <v>61</v>
+      <c r="B28" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" t="s">
         <v>69</v>
       </c>
-      <c r="D28" t="s">
-        <v>160</v>
-      </c>
-      <c r="E28" t="s">
-        <v>71</v>
-      </c>
       <c r="F28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C29" s="5"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -1694,322 +1685,322 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C33" s="5"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="34" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
-        <v>101</v>
+        <v>4</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="C34" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>175</v>
+      </c>
+      <c r="E34" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" t="s">
         <v>78</v>
       </c>
-      <c r="D34" t="s">
-        <v>161</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" t="s">
         <v>79</v>
       </c>
-      <c r="F34" t="s">
-        <v>80</v>
-      </c>
-      <c r="G34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" t="s">
-        <v>81</v>
-      </c>
       <c r="I34" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
-      <c r="B35" t="s">
-        <v>102</v>
+      <c r="B35" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="C35" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="E35" t="s">
-        <v>79</v>
-      </c>
-      <c r="F35" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" t="s">
-        <v>84</v>
-      </c>
       <c r="I35" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2</v>
       </c>
-      <c r="B36" t="s">
-        <v>103</v>
+      <c r="B36" s="12" t="s">
+        <v>101</v>
       </c>
       <c r="C36" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E36" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" t="s">
+        <v>84</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E36" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" t="s">
-        <v>86</v>
-      </c>
-      <c r="G36" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" t="s">
-        <v>87</v>
-      </c>
       <c r="I36" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
-      <c r="B37" t="s">
-        <v>98</v>
+      <c r="B37" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G37" t="s">
         <v>11</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>4</v>
-      </c>
-      <c r="B38" t="s">
-        <v>99</v>
+        <v>3</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G38" t="s">
         <v>11</v>
       </c>
       <c r="H38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I38" s="11"/>
       <c r="J38" s="11"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2</v>
       </c>
-      <c r="B39" t="s">
-        <v>100</v>
+      <c r="B39" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="C39" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" t="s">
+        <v>177</v>
+      </c>
+      <c r="E39" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" t="s">
         <v>90</v>
       </c>
-      <c r="D39" t="s">
-        <v>113</v>
-      </c>
-      <c r="E39" t="s">
-        <v>79</v>
-      </c>
-      <c r="F39" t="s">
-        <v>91</v>
-      </c>
-      <c r="G39" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D40" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G40" t="s">
         <v>11</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="E41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G41" t="s">
         <v>11</v>
       </c>
       <c r="H41" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="D42" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="E42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F42" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="G42" t="s">
         <v>11</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="D43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="G43" t="s">
         <v>11</v>
       </c>
       <c r="H43" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="D44" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="E44" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="G44" t="s">
         <v>11</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B45" s="7"/>
     </row>
   </sheetData>
@@ -2024,7 +2015,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>